<commit_message>
[v. 0.7.27a, de 20/09/2025]
</commit_message>
<xml_diff>
--- a/app_front/projeto/_agora_Dados Contabeis antigo p novo (AN)/dados_contabeis_finscore_TESTE_App_AN.xlsx
+++ b/app_front/projeto/_agora_Dados Contabeis antigo p novo (AN)/dados_contabeis_finscore_TESTE_App_AN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/Desktop OneDrive/FinScore/app_front/projeto/agora_Dados Contabeis antigo p novo (AN)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/Desktop OneDrive/FinScore/app_front/projeto/_agora_Dados Contabeis antigo p novo (AN)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{9C24A7FC-58AE-40AA-BE7E-0C105E25FF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3BB6D82-0C44-4858-B4B4-E76BF0F23F17}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9C24A7FC-58AE-40AA-BE7E-0C105E25FF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C31BE7-8AE6-4BF1-8245-64F41E956D60}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lancamentos" sheetId="1" r:id="rId1"/>
@@ -455,13 +455,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>

</xml_diff>